<commit_message>
Updade 1V ADC.brd enviada pra digikart
</commit_message>
<xml_diff>
--- a/NOTCH.xlsx
+++ b/NOTCH.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="75" windowWidth="11235" windowHeight="9375" activeTab="2"/>
+    <workbookView xWindow="90" yWindow="75" windowWidth="11235" windowHeight="9375" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Lista de materiais" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="144">
   <si>
     <t>C=</t>
   </si>
@@ -343,6 +344,111 @@
   </si>
   <si>
     <t>Embarcar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ponte de Wheatstone </t>
+  </si>
+  <si>
+    <t>Filtro 3Mhz</t>
+  </si>
+  <si>
+    <t>Controle automático de ganho</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>Avulsos</t>
+  </si>
+  <si>
+    <t>22k</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>4.7uf</t>
+  </si>
+  <si>
+    <t>100nf</t>
+  </si>
+  <si>
+    <t>1pf</t>
+  </si>
+  <si>
+    <t>10pf</t>
+  </si>
+  <si>
+    <t>3.3k</t>
+  </si>
+  <si>
+    <t>PoT 100k</t>
+  </si>
+  <si>
+    <t>6.8k</t>
+  </si>
+  <si>
+    <t>5.6k</t>
+  </si>
+  <si>
+    <t>12k</t>
+  </si>
+  <si>
+    <t>27k</t>
+  </si>
+  <si>
+    <t>LT6323</t>
+  </si>
+  <si>
+    <t>AD9288</t>
+  </si>
+  <si>
+    <t>AD5445</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumper </t>
+  </si>
+  <si>
+    <t>Barra pino(20x2)</t>
+  </si>
+  <si>
+    <t>Born alimentação</t>
+  </si>
+  <si>
+    <t>Barra pino (3x1)</t>
+  </si>
+  <si>
+    <t>1.5k</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>24k</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>12.7k</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>3.74k</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>x'</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
@@ -1524,4 +1630,384 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="D1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="B2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" t="s">
+        <v>117</v>
+      </c>
+      <c r="N2" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" t="s">
+        <v>128</v>
+      </c>
+      <c r="S2" t="s">
+        <v>129</v>
+      </c>
+      <c r="T2" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" t="s">
+        <v>132</v>
+      </c>
+      <c r="V2" t="s">
+        <v>130</v>
+      </c>
+      <c r="W2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+      <c r="M4" s="4">
+        <v>4</v>
+      </c>
+      <c r="N4" s="4">
+        <v>4</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>3</v>
+      </c>
+      <c r="K5" s="4">
+        <v>21</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4">
+        <v>3</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
+        <v>2</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4">
+        <v>1</v>
+      </c>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4">
+        <v>1</v>
+      </c>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4">
+        <v>2</v>
+      </c>
+      <c r="U8" s="4">
+        <v>6</v>
+      </c>
+      <c r="V8" s="4">
+        <v>3</v>
+      </c>
+      <c r="W8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
+      <c r="H10">
+        <v>6</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>45</v>
+      </c>
+      <c r="M10">
+        <v>8</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="V11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>